<commit_message>
1.fix bug in datascatter about 'nan' in set or list
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Weaver\Universa\MisesqEx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7275"/>
+    <workbookView windowWidth="19200" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="analy" sheetId="1" r:id="rId1"/>
@@ -178,7 +173,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>2</t>
     </r>
@@ -186,7 +181,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>021-03-31 00:00:00</t>
     </r>
@@ -198,15 +193,20 @@
     <t>2021-09-30 00:00:00</t>
   </si>
   <si>
-    <t>2022-01-20 00:00:00</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>2022-02-06 00:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -215,23 +215,355 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -239,9 +571,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -254,17 +828,61 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -522,354 +1140,352 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.70909090909091" defaultRowHeight="12.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="19.5703125" customWidth="1"/>
+    <col min="1" max="2" width="19.5727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
add new data to timeex
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>date</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>2020-09-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-31 00:00:00</t>
   </si>
   <si>
     <r>
@@ -193,7 +196,13 @@
     <t>2021-09-30 00:00:00</t>
   </si>
   <si>
-    <t>2022-02-06 00:00:00</t>
+    <t>2021-12-31 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-03-31 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-04-29 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -201,46 +210,64 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,25 +280,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,39 +311,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -339,9 +335,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -349,21 +352,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -384,181 +388,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,11 +593,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -609,6 +626,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,185 +665,163 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -826,7 +830,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1148,10 +1151,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.70909090909091" defaultRowHeight="12.5" outlineLevelCol="1"/>
@@ -1470,10 +1473,11 @@
       </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:2">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="3" t="s">
@@ -1481,8 +1485,23 @@
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.Incremental calculation and use misesqbase.xlsx as input
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Weaver\Universa\MisesqEx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7275"/>
+    <workbookView windowWidth="18530" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="analy" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>date</t>
   </si>
@@ -181,7 +176,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>2</t>
     </r>
@@ -189,7 +184,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>021-03-31 00:00:00</t>
     </r>
@@ -207,74 +202,378 @@
     <t>2022-03-31 00:00:00</t>
   </si>
   <si>
-    <r>
-      <t>2022-0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> 00:00:00</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>2022-06-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-09-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-10-31 00:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -282,11 +581,253 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -295,19 +836,62 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -565,370 +1149,378 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.70909090909091" defaultRowHeight="12.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="19.5703125" customWidth="1"/>
+    <col min="1" max="2" width="19.5727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+    <row r="58" spans="1:1">
+      <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
     </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
1.time and timeex update
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7270"/>
+    <workbookView windowWidth="18530" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="analy" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
     <t>2022-09-30 00:00:00</t>
   </si>
   <si>
-    <t>2022-12-12 00:00:00</t>
+    <t>2022-12-19 00:00:00</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
1.fixed some alarm like append()
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>date</t>
   </si>
@@ -208,7 +208,13 @@
     <t>2022-09-30 00:00:00</t>
   </si>
   <si>
-    <t>2022-12-19 00:00:00</t>
+    <t>2022-12-31 00:00:00</t>
+  </si>
+  <si>
+    <t>2023-03-31 00:00:00</t>
+  </si>
+  <si>
+    <t>2023-04-30 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -1157,10 +1163,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.70909090909091" defaultRowHeight="12.5" outlineLevelCol="1"/>
@@ -1520,6 +1526,16 @@
         <v>59</v>
       </c>
     </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>

<commit_message>
1.update conda and akshare 2.fix some bug in scatter
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -4,17 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7270"/>
+    <workbookView windowWidth="18350" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="analy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>date</t>
   </si>
@@ -220,13 +233,19 @@
     <t>2023-09-30 00:00:00</t>
   </si>
   <si>
-    <t>2023-12-11 00:00:00</t>
+    <t>2023-12-31 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-03-31 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-05-16 00:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -247,55 +266,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -340,6 +323,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -385,7 +383,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -400,49 +419,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,121 +557,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,21 +610,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -638,6 +642,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -694,148 +713,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -851,52 +870,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1169,10 +1188,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.70909090909091" defaultRowHeight="12.5" outlineLevelCol="1"/>
@@ -1552,6 +1571,16 @@
         <v>63</v>
       </c>
     </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>